<commit_message>
enhance target partition list
</commit_message>
<xml_diff>
--- a/dbx_context_param.xlsx
+++ b/dbx_context_param.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KLMembrano\OneDrive - PLDT\dbx_automation\dbx_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0A1CEE-762E-49D1-A20C-8C7AE837A3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A6F03B-A6F7-4CD3-97A2-9DEE851E9E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" activeTab="1" xr2:uid="{15E29264-49B0-4491-96C0-AFEF115122E3}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="183">
   <si>
     <t>iteration</t>
   </si>
@@ -457,18 +457,9 @@
     <t>subscriptionproperty</t>
   </si>
   <si>
-    <t>cox_nrt_acounthistory</t>
-  </si>
-  <si>
-    <t>GENZ - Bronze ingest  acounthistory</t>
-  </si>
-  <si>
     <t>/talend_prod/data/hive/gdm_landing/cox_nrt_acounthistory/</t>
   </si>
   <si>
-    <t>parquet</t>
-  </si>
-  <si>
     <t>cox*</t>
   </si>
   <si>
@@ -494,9 +485,6 @@
   </si>
   <si>
     <t>asd</t>
-  </si>
-  <si>
-    <t>daily</t>
   </si>
   <si>
     <t>p_retention_key</t>
@@ -629,6 +617,27 @@
   </si>
   <si>
     <t>DO NOT CHANGE</t>
+  </si>
+  <si>
+    <t>wiwe_vnt_subscriber_dly</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>GENZ - Bronze ingest  wiwe_vnt_subscriber_dly</t>
+  </si>
+  <si>
+    <t>file_timestamp_bucket</t>
+  </si>
+  <si>
+    <t>timestampbucket</t>
+  </si>
+  <si>
+    <t>daily</t>
   </si>
 </sst>
 </file>
@@ -1035,6 +1044,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1055,16 +1074,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1108,8 +1117,8 @@
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>1203960</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1632,8 +1641,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K131"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1643,7 +1652,7 @@
     <col min="3" max="3" width="12.09765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.69921875" style="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.09765625" customWidth="1"/>
-    <col min="9" max="9" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.3984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23.8984375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1662,10 +1671,10 @@
         <v>99</v>
       </c>
       <c r="E1" s="38" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F1" s="38" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1680,7 +1689,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E2" t="str" cm="1">
         <f t="array" ref="E2:F2">_xlfn.XLOOKUP(B2,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
@@ -1705,13 +1714,13 @@
         <v>_c1</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E3" t="str" cm="1">
         <f t="array" ref="E3">_xlfn.XLOOKUP(B3,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
@@ -1731,7 +1740,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E4" t="str" cm="1">
         <f t="array" ref="E4">_xlfn.XLOOKUP(B4,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
@@ -1769,14 +1778,14 @@
         <v>6</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E6" t="str" cm="1">
         <f t="array" ref="E6">_xlfn.XLOOKUP(B6,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
         <v/>
       </c>
       <c r="I6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J6" t="s">
         <v>110</v>
@@ -1794,10 +1803,10 @@
         <v>121</v>
       </c>
       <c r="C7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E7" t="str" cm="1">
         <f t="array" ref="E7">_xlfn.XLOOKUP(B7,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
@@ -1825,20 +1834,20 @@
         <v>6</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E8" t="str" cm="1">
         <f t="array" ref="E8">_xlfn.XLOOKUP(B8,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
         <v/>
       </c>
       <c r="I8" t="s">
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="J8" t="s">
         <v>101</v>
       </c>
       <c r="K8" t="s">
-        <v>114</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1853,20 +1862,20 @@
         <v>6</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E9" t="str" cm="1">
         <f t="array" ref="E9">_xlfn.XLOOKUP(B9,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
         <v/>
       </c>
       <c r="I9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J9" t="s">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="K9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1881,20 +1890,20 @@
         <v>6</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E10" t="str" cm="1">
         <f t="array" ref="E10">_xlfn.XLOOKUP(B10,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
         <v/>
       </c>
       <c r="I10" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
       <c r="J10" t="s">
         <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>5</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1909,11 +1918,20 @@
         <v>6</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E11" t="str" cm="1">
         <f t="array" ref="E11">_xlfn.XLOOKUP(B11,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
         <v/>
+      </c>
+      <c r="I11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1928,7 +1946,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E12" t="str" cm="1">
         <f t="array" ref="E12">_xlfn.XLOOKUP(B12,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
@@ -1963,7 +1981,7 @@
         <v>_c12</v>
       </c>
       <c r="B14" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
         <v>110</v>
@@ -1982,7 +2000,7 @@
         <v>_c13</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C15" t="s">
         <v>101</v>
@@ -2007,7 +2025,7 @@
         <v>6</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E16" t="str" cm="1">
         <f t="array" ref="E16:F16">_xlfn.XLOOKUP(B16,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
@@ -2029,7 +2047,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E17" t="str" cm="1">
         <f t="array" ref="E17:F17">_xlfn.XLOOKUP(B17,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
@@ -2064,7 +2082,7 @@
         <v>_c17</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C19" t="s">
         <v>110</v>
@@ -2083,7 +2101,7 @@
         <v>_c18</v>
       </c>
       <c r="B20" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C20" t="s">
         <v>101</v>
@@ -2105,13 +2123,13 @@
         <v>_c19</v>
       </c>
       <c r="B21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E21" t="str" cm="1">
         <f t="array" ref="E21">_xlfn.XLOOKUP(B21,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
@@ -2124,13 +2142,13 @@
         <v>_c20</v>
       </c>
       <c r="B22" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E22" t="str" cm="1">
         <f t="array" ref="E22">_xlfn.XLOOKUP(B22,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
@@ -2162,13 +2180,13 @@
         <v>_c22</v>
       </c>
       <c r="B24" t="s">
-        <v>109</v>
+        <v>180</v>
       </c>
       <c r="C24" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E24" t="str" cm="1">
         <f t="array" ref="E24">_xlfn.XLOOKUP(B24,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
@@ -2206,7 +2224,7 @@
         <v>6</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E26" t="str" cm="1">
         <f t="array" ref="E26">_xlfn.XLOOKUP(B26,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
@@ -2225,7 +2243,7 @@
         <v>6</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E27" t="str" cm="1">
         <f t="array" ref="E27">_xlfn.XLOOKUP(B27,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
@@ -2758,18 +2776,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId4" name="removeSpace_comma">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+        <control shapeId="1025" r:id="rId4" name="lowerCase">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>10</xdr:col>
+                <xdr:col>8</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>11</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>1203960</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -2778,7 +2796,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1029" r:id="rId4" name="removeSpace_comma"/>
+        <control shapeId="1025" r:id="rId4" name="lowerCase"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2808,17 +2826,17 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId8" name="lowerCase">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
+        <control shapeId="1029" r:id="rId8" name="removeSpace_comma">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>8</xdr:col>
+                <xdr:col>10</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>9</xdr:col>
+                <xdr:col>11</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
@@ -2828,7 +2846,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId8" name="lowerCase"/>
+        <control shapeId="1029" r:id="rId8" name="removeSpace_comma"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -2841,7 +2859,7 @@
   <dimension ref="B3:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2861,10 +2879,10 @@
       <c r="C3" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="50" t="s">
-        <v>173</v>
-      </c>
-      <c r="G3" s="51"/>
+      <c r="F3" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="G3" s="44"/>
     </row>
     <row r="4" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
@@ -2875,115 +2893,117 @@
         <v>_b</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>123</v>
+      <c r="C5" s="41" t="s">
+        <v>176</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="F6" s="49" t="s">
-        <v>176</v>
+      <c r="F6" s="42" t="s">
+        <v>172</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="48" t="s">
-        <v>123</v>
+      <c r="C7" s="41" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="41" t="s">
         <v>106</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="48" t="s">
-        <v>136</v>
+      <c r="C9" s="41" t="s">
+        <v>182</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G9" s="40" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="48" t="s">
-        <v>126</v>
+      <c r="C10" s="41" t="s">
+        <v>177</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="48" t="b">
+      <c r="C11" s="41" t="b">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G11" s="39" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="48"/>
+      <c r="C12" s="41" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="41" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2991,64 +3011,66 @@
       <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="48" t="s">
-        <v>125</v>
+      <c r="C14" s="41" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="48" t="s">
-        <v>127</v>
+      <c r="C15" s="41" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="48" t="s">
-        <v>129</v>
+      <c r="C16" s="41" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="48" t="s">
-        <v>124</v>
+      <c r="C17" s="41" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C18" s="32" t="str">
         <f>_xlfn.CONCAT(D18,"_task")</f>
-        <v>cox_nrt_acounthistory_task</v>
+        <v>wiwe_vnt_subscriber_dly_task</v>
       </c>
       <c r="D18" s="36" t="str">
         <f>C7</f>
-        <v>cox_nrt_acounthistory</v>
+        <v>wiwe_vnt_subscriber_dly</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C19" s="32" t="str">
         <f>IF(LOWER(C9)="hourly","file_timestamp_bucket, txn_date",
-   IF(LOWER(C9)="daily","txn_date, file_date",""))</f>
+IF(LOWER(C9)="daily","txn_date, file_date",
+IF(LOWER(C9)="minutes","file_timestamp_bucket, txn_date","")))</f>
         <v>txn_date, file_date</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="34" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C20" s="35" t="str">
         <f>IF(LOWER(C9)="hourly","file_timestamp_bucket",
-   IF(LOWER(C9)="daily","txn_date",""))</f>
+IF(LOWER(C9)="daily","txn_date",
+IF(LOWER(C9)="minutes","file_timestamp_bucket","")))</f>
         <v>txn_date</v>
       </c>
     </row>
@@ -3057,6 +3079,7 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3077,13 +3100,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3091,10 +3114,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3102,10 +3125,10 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3113,10 +3136,10 @@
         <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3124,21 +3147,21 @@
         <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -3146,10 +3169,10 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -3157,219 +3180,219 @@
         <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B9" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B10" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C10" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C12" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B13" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B14" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C15" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B16" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C16" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B17" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B18" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C18" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B19" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C19" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B20" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C20" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B21" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C21" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B22" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C22" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B23" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C23" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B24" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C24" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B25" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C25" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B26" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C26" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B27" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C27" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -3377,10 +3400,10 @@
         <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C28" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -3388,10 +3411,10 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C29" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -3829,19 +3852,19 @@
     <row r="24" spans="1:4" s="21" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
-        <v>22,file_date</v>
+        <v>22,file_timestamp_bucket</v>
       </c>
       <c r="B24" s="21" t="str">
         <f>IF(schema!B24&lt;&gt;"", schema!B24, "")</f>
-        <v>file_date</v>
+        <v>file_timestamp_bucket</v>
       </c>
       <c r="C24" s="21" t="str">
         <f>IF(schema!C24&lt;&gt;"", schema!C24, "")</f>
-        <v>date</v>
+        <v>timestamp</v>
       </c>
       <c r="D24" s="20" t="str">
         <f>IF(schema!B24&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B24), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B24, 0),"")</f>
-        <v>file_date</v>
+        <v>file_timestamp_bucket</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="21" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -7665,10 +7688,10 @@
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="48" t="s">
         <v>67</v>
       </c>
       <c r="G8" s="11" t="s">
@@ -7688,8 +7711,8 @@
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
       <c r="G9" s="11" t="s">
         <v>71</v>
       </c>
@@ -7722,10 +7745,10 @@
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="44" t="s">
+      <c r="E11" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="44" t="s">
+      <c r="F11" s="48" t="s">
         <v>74</v>
       </c>
       <c r="G11" s="11" t="s">
@@ -7745,8 +7768,8 @@
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
       <c r="G12" s="11" t="s">
         <v>71</v>
       </c>
@@ -7871,10 +7894,10 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="44" t="s">
+      <c r="E20" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="46" t="s">
+      <c r="F20" s="50" t="s">
         <v>80</v>
       </c>
       <c r="G20" s="11" t="s">
@@ -7894,8 +7917,8 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="47"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="51"/>
       <c r="G21" s="11" t="s">
         <v>71</v>
       </c>
@@ -7941,14 +7964,14 @@
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="41" t="s">
+      <c r="E24" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="43"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="47"/>
       <c r="K24" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added talend schema xml convert to ddl
</commit_message>
<xml_diff>
--- a/dbx_context_param.xlsx
+++ b/dbx_context_param.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KLMembrano\OneDrive - PLDT\dbx_automation\dbx_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911A66A2-35B0-40E6-BFC4-1ED08214B84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF18157-63B4-4F58-8F2A-2C40EA3827C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" xr2:uid="{15E29264-49B0-4491-96C0-AFEF115122E3}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="178">
   <si>
     <t>iteration</t>
   </si>
@@ -620,6 +620,9 @@
   </si>
   <si>
     <t>sid_source</t>
+  </si>
+  <si>
+    <t>bigdecimal</t>
   </si>
 </sst>
 </file>
@@ -1624,7 +1627,7 @@
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1670,7 +1673,9 @@
       <c r="C2" t="s">
         <v>168</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="28" t="s">
+        <v>177</v>
+      </c>
       <c r="E2" t="str" cm="1">
         <f t="array" ref="E2">_xlfn.XLOOKUP(B2,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
         <v/>
@@ -2623,18 +2628,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="lowerCase">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="1029" r:id="rId4" name="removeSpace_comma">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>8</xdr:col>
+                <xdr:col>10</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>1203960</xdr:colOff>
+                <xdr:col>11</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -2643,7 +2648,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="lowerCase"/>
+        <control shapeId="1029" r:id="rId4" name="removeSpace_comma"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2673,18 +2678,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId8" name="removeSpace_comma">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+        <control shapeId="1025" r:id="rId8" name="lowerCase">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>10</xdr:col>
+                <xdr:col>8</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>11</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>1203960</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -2693,7 +2698,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1029" r:id="rId8" name="removeSpace_comma"/>
+        <control shapeId="1025" r:id="rId8" name="lowerCase"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
update delimiter for xml_to_ddl.py
</commit_message>
<xml_diff>
--- a/dbx_context_param.xlsx
+++ b/dbx_context_param.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KLMembrano\OneDrive - PLDT\dbx_automation\dbx_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF18157-63B4-4F58-8F2A-2C40EA3827C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73496F04-2CC6-48D3-A402-C7F474A12245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" xr2:uid="{15E29264-49B0-4491-96C0-AFEF115122E3}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="180">
   <si>
     <t>iteration</t>
   </si>
@@ -428,9 +428,6 @@
   </si>
   <si>
     <t>p_task_key_name</t>
-  </si>
-  <si>
-    <t>4gb</t>
   </si>
   <si>
     <t>txn_date</t>
@@ -580,49 +577,58 @@
     <t>daily</t>
   </si>
   <si>
-    <t>optima_daily_cb_procinstextid</t>
-  </si>
-  <si>
     <t>parquet</t>
   </si>
   <si>
-    <t>procinstextid*</t>
-  </si>
-  <si>
-    <t>/talend_prod/data/hive/gdm_landing/optima/procinstextid/</t>
-  </si>
-  <si>
-    <t>OPTIMA - optima_daily_cb_procinstextid</t>
-  </si>
-  <si>
-    <t>bigint</t>
-  </si>
-  <si>
-    <t>accountinternalid</t>
-  </si>
-  <si>
-    <t>assigneeroleid</t>
-  </si>
-  <si>
-    <t>externalid</t>
-  </si>
-  <si>
-    <t>processinstdocid</t>
-  </si>
-  <si>
-    <t>sladuedate</t>
-  </si>
-  <si>
-    <t>slathresholddate</t>
-  </si>
-  <si>
-    <t>tenantid</t>
-  </si>
-  <si>
     <t>sid_source</t>
   </si>
   <si>
-    <t>bigdecimal</t>
+    <t>opt_dly_descriptions</t>
+  </si>
+  <si>
+    <t>/talend_prod/data/hive/gdm_landing/optima/opt_dly_descriptions/</t>
+  </si>
+  <si>
+    <t>opt_dly_descriptions*</t>
+  </si>
+  <si>
+    <t>1gb</t>
+  </si>
+  <si>
+    <t>OPTIMA - opt_dly_descriptions</t>
+  </si>
+  <si>
+    <t>description_code</t>
+  </si>
+  <si>
+    <t>language_code</t>
+  </si>
+  <si>
+    <t>double(10,0)</t>
+  </si>
+  <si>
+    <t>double(6,0)</t>
+  </si>
+  <si>
+    <t>description_group</t>
+  </si>
+  <si>
+    <t>description_text</t>
+  </si>
+  <si>
+    <t>short_description_text</t>
+  </si>
+  <si>
+    <t>config_tag_id</t>
+  </si>
+  <si>
+    <t>tenant_id</t>
+  </si>
+  <si>
+    <t>process_dt</t>
+  </si>
+  <si>
+    <t>dd-MM-yyyy</t>
   </si>
 </sst>
 </file>
@@ -1627,7 +1633,7 @@
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1656,10 +1662,10 @@
         <v>99</v>
       </c>
       <c r="E1" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="38" t="s">
         <v>119</v>
-      </c>
-      <c r="F1" s="38" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1671,11 +1677,9 @@
         <v>169</v>
       </c>
       <c r="C2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>177</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="D2" s="28"/>
       <c r="E2" t="str" cm="1">
         <f t="array" ref="E2">_xlfn.XLOOKUP(B2,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
         <v/>
@@ -1699,7 +1703,7 @@
         <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
       <c r="D3" s="28"/>
       <c r="E3" t="str" cm="1">
@@ -1714,10 +1718,10 @@
         <v>_c2</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
       <c r="D4" s="29"/>
       <c r="E4" t="str" cm="1">
@@ -1731,10 +1735,10 @@
         <v>_c3</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C5" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" t="str" cm="1">
@@ -1748,7 +1752,7 @@
         <v>_c4</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -1759,7 +1763,7 @@
         <v/>
       </c>
       <c r="I6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J6" t="s">
         <v>108</v>
@@ -1774,7 +1778,7 @@
         <v>_c5</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -1800,10 +1804,10 @@
         <v>_c6</v>
       </c>
       <c r="B8" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="D8" s="29"/>
       <c r="E8" t="str" cm="1">
@@ -1811,13 +1815,13 @@
         <v/>
       </c>
       <c r="I8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J8" t="s">
         <v>101</v>
       </c>
       <c r="K8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1826,7 +1830,7 @@
         <v>_c7</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -1852,13 +1856,13 @@
         <v>_c8</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>178</v>
       </c>
       <c r="C10" t="s">
         <v>108</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>179</v>
       </c>
       <c r="E10" t="str" cm="1">
         <f t="array" ref="E10">_xlfn.XLOOKUP(B10,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
@@ -1877,17 +1881,9 @@
     <row r="11" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f t="shared" si="1"/>
-        <v>_c9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" t="s">
-        <v>110</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D11"/>
       <c r="E11" t="str" cm="1">
         <f t="array" ref="E11">_xlfn.XLOOKUP(B11,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
         <v/>
@@ -1905,17 +1901,9 @@
     <row r="12" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f t="shared" si="1"/>
-        <v>_c10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D12" t="s">
-        <v>111</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D12"/>
       <c r="E12" t="str" cm="1">
         <f t="array" ref="E12">_xlfn.XLOOKUP(B12,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
         <v/>
@@ -1924,17 +1912,9 @@
     <row r="13" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f t="shared" si="1"/>
-        <v>_c11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>112</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D13"/>
       <c r="E13" t="str" cm="1">
         <f t="array" ref="E13">_xlfn.XLOOKUP(B13,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
         <v/>
@@ -1943,17 +1923,9 @@
     <row r="14" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f t="shared" si="1"/>
-        <v>_c12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D14"/>
       <c r="E14" t="str" cm="1">
         <f t="array" ref="E14">_xlfn.XLOOKUP(B14,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
         <v/>
@@ -2628,18 +2600,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId4" name="removeSpace_comma">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+        <control shapeId="1025" r:id="rId4" name="lowerCase">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>10</xdr:col>
+                <xdr:col>8</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>11</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>1203960</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -2648,7 +2620,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1029" r:id="rId4" name="removeSpace_comma"/>
+        <control shapeId="1025" r:id="rId4" name="lowerCase"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2678,18 +2650,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId8" name="lowerCase">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
+        <control shapeId="1029" r:id="rId8" name="removeSpace_comma">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>8</xdr:col>
+                <xdr:col>10</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>1203960</xdr:colOff>
+                <xdr:col>11</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -2698,7 +2670,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId8" name="lowerCase"/>
+        <control shapeId="1029" r:id="rId8" name="removeSpace_comma"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -2711,13 +2683,13 @@
   <dimension ref="B3:G20"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.796875" customWidth="1"/>
-    <col min="3" max="3" width="49.296875" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5" style="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.296875" customWidth="1"/>
     <col min="5" max="5" width="1.19921875" customWidth="1"/>
     <col min="6" max="6" width="18.19921875" bestFit="1" customWidth="1"/>
@@ -2732,7 +2704,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="43" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G3" s="44"/>
     </row>
@@ -2745,10 +2717,10 @@
         <v>_b</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
@@ -2756,13 +2728,13 @@
         <v>8</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
@@ -2773,10 +2745,10 @@
         <v>106</v>
       </c>
       <c r="F6" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
@@ -2784,7 +2756,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
@@ -2795,10 +2767,10 @@
         <v>104</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2806,13 +2778,13 @@
         <v>9</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G9" s="40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
@@ -2820,13 +2792,13 @@
         <v>17</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
@@ -2837,10 +2809,10 @@
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G11" s="39" t="s">
         <v>150</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
@@ -2862,7 +2834,7 @@
         <v>19</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
@@ -2870,7 +2842,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
@@ -2878,7 +2850,7 @@
         <v>103</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>114</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
@@ -2886,7 +2858,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
@@ -2895,16 +2867,16 @@
       </c>
       <c r="C18" s="32" t="str">
         <f>_xlfn.CONCAT(D18,"_task")</f>
-        <v>optima_daily_cb_procinstextid_task</v>
+        <v>opt_dly_descriptions_task</v>
       </c>
       <c r="D18" s="36" t="str">
         <f>C7</f>
-        <v>optima_daily_cb_procinstextid</v>
+        <v>opt_dly_descriptions</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C19" s="32" t="str">
         <f>IF(LOWER(C9)="hourly","file_timestamp_bucket, txn_date",
@@ -2915,7 +2887,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C20" s="35" t="str">
         <f>IF(LOWER(C9)="hourly","file_timestamp_bucket",
@@ -2951,13 +2923,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="C1" s="37" t="s">
         <v>119</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2965,10 +2937,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" t="s">
         <v>121</v>
-      </c>
-      <c r="C2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2976,10 +2948,10 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" t="s">
         <v>121</v>
-      </c>
-      <c r="C3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2987,10 +2959,10 @@
         <v>88</v>
       </c>
       <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
         <v>121</v>
-      </c>
-      <c r="C4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2998,21 +2970,21 @@
         <v>89</v>
       </c>
       <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" t="s">
         <v>121</v>
-      </c>
-      <c r="C5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" t="s">
         <v>121</v>
-      </c>
-      <c r="C6" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -3020,10 +2992,10 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" t="s">
         <v>121</v>
-      </c>
-      <c r="C7" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -3031,219 +3003,219 @@
         <v>37</v>
       </c>
       <c r="B8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" t="s">
         <v>121</v>
-      </c>
-      <c r="C8" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" t="s">
         <v>121</v>
-      </c>
-      <c r="C9" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" t="s">
         <v>121</v>
-      </c>
-      <c r="C10" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" t="s">
         <v>121</v>
-      </c>
-      <c r="C11" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" t="s">
         <v>121</v>
-      </c>
-      <c r="C12" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" t="s">
         <v>121</v>
-      </c>
-      <c r="C13" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" t="s">
         <v>121</v>
-      </c>
-      <c r="C14" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" t="s">
         <v>121</v>
-      </c>
-      <c r="C15" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" t="s">
         <v>121</v>
-      </c>
-      <c r="C16" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" t="s">
         <v>121</v>
-      </c>
-      <c r="C17" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18" t="s">
         <v>133</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>134</v>
-      </c>
-      <c r="C18" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" t="s">
         <v>134</v>
-      </c>
-      <c r="C19" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" t="s">
         <v>134</v>
-      </c>
-      <c r="C20" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C21" t="s">
         <v>134</v>
-      </c>
-      <c r="C21" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" t="s">
         <v>134</v>
-      </c>
-      <c r="C22" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" t="s">
         <v>134</v>
-      </c>
-      <c r="C23" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B24" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" t="s">
         <v>134</v>
-      </c>
-      <c r="C24" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" t="s">
         <v>134</v>
-      </c>
-      <c r="C25" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C26" t="s">
         <v>134</v>
-      </c>
-      <c r="C26" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B27" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" t="s">
         <v>134</v>
-      </c>
-      <c r="C27" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -3251,10 +3223,10 @@
         <v>55</v>
       </c>
       <c r="B28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C28" t="s">
         <v>134</v>
-      </c>
-      <c r="C28" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -3262,10 +3234,10 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" t="s">
         <v>134</v>
-      </c>
-      <c r="C29" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -3307,83 +3279,83 @@
     <row r="2" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>IF(B2&lt;&gt;"", ROW(B2)-ROW($B$2) &amp; ","&amp;B2, "")</f>
-        <v>0,accountinternalid</v>
+        <v>0,description_code</v>
       </c>
       <c r="B2" t="str">
         <f>IF(schema!B2&lt;&gt;"", schema!B2, "")</f>
-        <v>accountinternalid</v>
+        <v>description_code</v>
       </c>
       <c r="C2" t="str">
         <f>IF(schema!C2&lt;&gt;"", schema!C2, "")</f>
-        <v>bigint</v>
+        <v>double(10,0)</v>
       </c>
       <c r="D2" s="20" t="str">
         <f>IF(schema!B2&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B2), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B2, 0),"")</f>
-        <v>accountinternalid</v>
+        <v>description_code</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A66" si="0">IF(B3&lt;&gt;"", ROW(B3)-ROW($B$2) &amp; ","&amp;B3, "")</f>
-        <v>1,assigneeroleid</v>
+        <v>1,language_code</v>
       </c>
       <c r="B3" t="str">
         <f>IF(schema!B3&lt;&gt;"", schema!B3, "")</f>
-        <v>assigneeroleid</v>
+        <v>language_code</v>
       </c>
       <c r="C3" t="str">
         <f>IF(schema!C3&lt;&gt;"", schema!C3, "")</f>
-        <v>string</v>
+        <v>double(6,0)</v>
       </c>
       <c r="D3" s="20" t="str">
         <f>IF(schema!B3&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B3), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B3, 0),"")</f>
-        <v>assigneeroleid</v>
+        <v>language_code</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
-        <v>2,externalid</v>
+        <v>2,description_group</v>
       </c>
       <c r="B4" t="str">
         <f>IF(schema!B4&lt;&gt;"", schema!B4, "")</f>
-        <v>externalid</v>
+        <v>description_group</v>
       </c>
       <c r="C4" t="str">
         <f>IF(schema!C4&lt;&gt;"", schema!C4, "")</f>
-        <v>string</v>
+        <v>double(6,0)</v>
       </c>
       <c r="D4" s="20" t="str">
         <f>IF(schema!B4&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B4), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B4, 0),"")</f>
-        <v>externalid</v>
+        <v>description_group</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>3,processinstdocid</v>
+        <v>3,description_text</v>
       </c>
       <c r="B5" t="str">
         <f>IF(schema!B5&lt;&gt;"", schema!B5, "")</f>
-        <v>processinstdocid</v>
+        <v>description_text</v>
       </c>
       <c r="C5" t="str">
         <f>IF(schema!C5&lt;&gt;"", schema!C5, "")</f>
-        <v>bigint</v>
+        <v>string</v>
       </c>
       <c r="D5" s="20" t="str">
         <f>IF(schema!B5&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B5), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B5, 0),"")</f>
-        <v>processinstdocid</v>
+        <v>description_text</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
-        <v>4,sladuedate</v>
+        <v>4,short_description_text</v>
       </c>
       <c r="B6" t="str">
         <f>IF(schema!B6&lt;&gt;"", schema!B6, "")</f>
-        <v>sladuedate</v>
+        <v>short_description_text</v>
       </c>
       <c r="C6" t="str">
         <f>IF(schema!C6&lt;&gt;"", schema!C6, "")</f>
@@ -3391,17 +3363,17 @@
       </c>
       <c r="D6" s="20" t="str">
         <f>IF(schema!B6&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B6), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B6, 0),"")</f>
-        <v>sladuedate</v>
+        <v>short_description_text</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>5,slathresholddate</v>
+        <v>5,config_tag_id</v>
       </c>
       <c r="B7" t="str">
         <f>IF(schema!B7&lt;&gt;"", schema!B7, "")</f>
-        <v>slathresholddate</v>
+        <v>config_tag_id</v>
       </c>
       <c r="C7" t="str">
         <f>IF(schema!C7&lt;&gt;"", schema!C7, "")</f>
@@ -3409,25 +3381,25 @@
       </c>
       <c r="D7" s="20" t="str">
         <f>IF(schema!B7&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B7), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B7, 0),"")</f>
-        <v>slathresholddate</v>
+        <v>config_tag_id</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
-        <v>6,tenantid</v>
+        <v>6,tenant_id</v>
       </c>
       <c r="B8" t="str">
         <f>IF(schema!B8&lt;&gt;"", schema!B8, "")</f>
-        <v>tenantid</v>
+        <v>tenant_id</v>
       </c>
       <c r="C8" t="str">
         <f>IF(schema!C8&lt;&gt;"", schema!C8, "")</f>
-        <v>string</v>
+        <v>double(10,0)</v>
       </c>
       <c r="D8" s="20" t="str">
         <f>IF(schema!B8&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B8), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B8, 0),"")</f>
-        <v>tenantid</v>
+        <v>tenant_id</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -3451,11 +3423,11 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>8,txn_date</v>
+        <v>8,process_dt</v>
       </c>
       <c r="B10" t="str">
         <f>IF(schema!B10&lt;&gt;"", schema!B10, "")</f>
-        <v>txn_date</v>
+        <v>process_dt</v>
       </c>
       <c r="C10" t="str">
         <f>IF(schema!C10&lt;&gt;"", schema!C10, "")</f>
@@ -3463,79 +3435,79 @@
       </c>
       <c r="D10" s="20" t="str">
         <f>IF(schema!B10&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B10), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B10, 0),"")</f>
-        <v>txn_date</v>
+        <v>process_dt</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
-        <v>9,file_date</v>
+        <v/>
       </c>
       <c r="B11" t="str">
         <f>IF(schema!B11&lt;&gt;"", schema!B11, "")</f>
-        <v>file_date</v>
+        <v/>
       </c>
       <c r="C11" t="str">
         <f>IF(schema!C11&lt;&gt;"", schema!C11, "")</f>
-        <v>date</v>
+        <v/>
       </c>
       <c r="D11" s="20" t="str">
         <f>IF(schema!B11&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B11), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B11, 0),"")</f>
-        <v>file_date</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
-        <v>10,dbx_process_dttm</v>
+        <v/>
       </c>
       <c r="B12" t="str">
         <f>IF(schema!B12&lt;&gt;"", schema!B12, "")</f>
-        <v>dbx_process_dttm</v>
+        <v/>
       </c>
       <c r="C12" t="str">
         <f>IF(schema!C12&lt;&gt;"", schema!C12, "")</f>
-        <v>timestamp</v>
+        <v/>
       </c>
       <c r="D12" s="20" t="str">
         <f>IF(schema!B12&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B12), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B12, 0),"")</f>
-        <v>dbx_process_dttm</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>11,file_name</v>
+        <v/>
       </c>
       <c r="B13" t="str">
         <f>IF(schema!B13&lt;&gt;"", schema!B13, "")</f>
-        <v>file_name</v>
+        <v/>
       </c>
       <c r="C13" t="str">
         <f>IF(schema!C13&lt;&gt;"", schema!C13, "")</f>
-        <v>string</v>
+        <v/>
       </c>
       <c r="D13" s="20" t="str">
         <f>IF(schema!B13&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B13), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B13, 0),"")</f>
-        <v>file_name</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
-        <v>12,file_id</v>
+        <v/>
       </c>
       <c r="B14" t="str">
         <f>IF(schema!B14&lt;&gt;"", schema!B14, "")</f>
-        <v>file_id</v>
+        <v/>
       </c>
       <c r="C14" t="str">
         <f>IF(schema!C14&lt;&gt;"", schema!C14, "")</f>
-        <v>string</v>
+        <v/>
       </c>
       <c r="D14" s="20" t="str">
         <f>IF(schema!B14&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B14), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B14, 0),"")</f>
-        <v>file_id</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>